<commit_message>
Agrego recalculo de indicadores por Barrio.
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="70">
   <si>
     <t>link</t>
   </si>
@@ -69,9 +69,6 @@
     <t>transporte</t>
   </si>
   <si>
-    <t>barrios_censo_2011.zip</t>
-  </si>
-  <si>
     <t>comunas_caba_censo_2010.zip</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>http://data.buenosaires.gob.ar/dataset/subte-estaciones</t>
+  </si>
+  <si>
+    <t>barrios.zip</t>
+  </si>
+  <si>
+    <t>https://recursos-data.buenosaires.gob.ar/ckan2/barrios/barrios.zip</t>
+  </si>
+  <si>
+    <t>http://data.buenosaires.gob.ar/dataset/barrios</t>
   </si>
 </sst>
 </file>
@@ -660,8 +666,8 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -684,13 +690,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -698,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -707,10 +713,10 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -718,7 +724,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -727,10 +733,10 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -744,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -752,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -761,10 +767,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -772,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -781,10 +787,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -792,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -801,10 +807,10 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -812,7 +818,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -821,10 +827,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -838,7 +844,7 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -846,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -855,10 +861,10 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -866,7 +872,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -875,113 +881,119 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -990,12 +1002,12 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1004,12 +1016,12 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1018,12 +1030,12 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1032,12 +1044,12 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1046,12 +1058,12 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -1060,12 +1072,12 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1074,12 +1086,12 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1088,12 +1100,12 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1102,12 +1114,12 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1116,12 +1128,12 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -1130,12 +1142,12 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1144,12 +1156,12 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1158,12 +1170,12 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -1172,12 +1184,12 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -1186,81 +1198,81 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
         <v>42</v>
       </c>
-      <c r="C35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" t="s">
-        <v>43</v>
-      </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego notebook para descargar todos los recursos del archivo Links.xlsx
</commit_message>
<xml_diff>
--- a/Links.xlsx
+++ b/Links.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>link</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>data</t>
-  </si>
-  <si>
-    <t>documentacion</t>
   </si>
   <si>
     <t>http://data.buenosaires.gob.ar/dataset/colectivos</t>
@@ -700,7 +697,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -722,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
@@ -733,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -742,7 +739,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -750,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -759,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -767,7 +764,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -776,7 +773,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -784,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -793,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -801,7 +798,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -810,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -818,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -827,7 +824,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -835,7 +832,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -844,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -852,7 +849,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -861,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -869,7 +866,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -878,15 +875,15 @@
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -895,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -903,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -912,15 +909,15 @@
         <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -929,7 +926,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -937,7 +934,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -946,7 +943,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -954,7 +951,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -963,7 +960,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -971,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -980,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -988,7 +985,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -997,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1005,7 +1002,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1014,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1022,7 +1019,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1031,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1039,7 +1036,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1048,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1056,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1065,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1073,7 +1070,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1082,52 +1079,49 @@
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>